<commit_message>
integrando workflow para githubaction
</commit_message>
<xml_diff>
--- a/tasas-transfi.xlsx
+++ b/tasas-transfi.xlsx
@@ -1116,10 +1116,10 @@
         <v/>
       </c>
       <c r="N10" s="23" t="n">
-        <v>69</v>
+        <v>64.744</v>
       </c>
       <c r="O10" t="n">
-        <v>4261.01</v>
+        <v>4259</v>
       </c>
     </row>
     <row r="11">
@@ -1144,10 +1144,10 @@
     </row>
     <row r="12">
       <c r="N12" t="n">
-        <v>4291.8</v>
+        <v>4299</v>
       </c>
       <c r="O12" s="23" t="n">
-        <v>63</v>
+        <v>62.36</v>
       </c>
     </row>
     <row r="13" ht="15" customHeight="1" s="44" thickBot="1">

</xml_diff>

<commit_message>
Actualización automática de tasas-transfi.xlsx
</commit_message>
<xml_diff>
--- a/tasas-transfi.xlsx
+++ b/tasas-transfi.xlsx
@@ -1116,10 +1116,10 @@
         <v/>
       </c>
       <c r="N10" s="23" t="n">
-        <v>65</v>
+        <v>64.72</v>
       </c>
       <c r="O10" t="n">
-        <v>4263.99</v>
+        <v>4260.01</v>
       </c>
     </row>
     <row r="11">
@@ -1144,7 +1144,7 @@
     </row>
     <row r="12">
       <c r="N12" t="n">
-        <v>4289.9</v>
+        <v>4280</v>
       </c>
       <c r="O12" s="23" t="n">
         <v>63.82</v>

</xml_diff>